<commit_message>
Update Dummy Data, Bootstrap, and app.py
UPDATES:
- Added dummy data for showcase (current total = 15 data).
- Upgrade Bootstrap from v4.6 to v5.1.
- Update main_layout.html to properly use Bootstrap v5.1.
- Added docstring to app.py to better describe the functionality
  of each custom function.
</commit_message>
<xml_diff>
--- a/discussion_dummy_data.xlsx
+++ b/discussion_dummy_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\Programming_Project\Python\Python_Flask\bangkit_discussion_search_engine_showcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB22613-1231-4716-8735-272FFD59F1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB253E73-DE18-4EDF-9413-D7291D899B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10404" yWindow="1980" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>title</t>
   </si>
@@ -36,31 +36,139 @@
     <t>keywords</t>
   </si>
   <si>
-    <t>title 1</t>
-  </si>
-  <si>
-    <t>title 2</t>
-  </si>
-  <si>
-    <t>title 3</t>
-  </si>
-  <si>
-    <t>content 1: Lorem Ipsum is simply dummy text of the printing and typesetting industry. Lorem Ipsum has been the industry's standard dummy text ever since the 1500s, when an unknown printer took a galley of type and scrambled it to make a type specimen book. It has survived not only five centuries, but also the leap into electronic typesetting, remaining essentially unchanged. It was popularised in the 1960s with the release of Letraset sheets containing Lorem Ipsum passages, and more recently with desktop publishing software like Aldus PageMaker including versions of Lorem Ipsum.</t>
-  </si>
-  <si>
-    <t>content 2: It is a long established fact that a reader will be distracted by the readable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English. Many desktop publishing packages and web page editors now use Lorem Ipsum as their default model text, and a search for 'lorem ipsum' will uncover many web sites still in their infancy. Various versions have evolved over the years, sometimes by accident, sometimes on purpose (injected humour and the like).</t>
-  </si>
-  <si>
-    <t>content 3: here are many variations of passages of Lorem Ipsum available, but the majority have suffered alteration in some form, by injected humour, or randomised words which don't look even slightly believable. If you are going to use a passage of Lorem Ipsum, you need to be sure there isn't anything embarrassing hidden in the middle of text. All the Lorem Ipsum generators on the Internet tend to repeat predefined chunks as necessary, making this the first true generator on the Internet. It uses a dictionary of over 200 Latin words, combined with a handful of model sentence structures, to generate Lorem Ipsum which looks reasonable. The generated Lorem Ipsum is therefore always free from repetition, injected humour, or non-characteristic words etc.</t>
-  </si>
-  <si>
-    <t>keywordfaef, keyword, keywordfa</t>
-  </si>
-  <si>
-    <t>keywordef, keywordaef, keywordfe</t>
-  </si>
-  <si>
-    <t>keywordfe, keywordugu,         keyword</t>
+    <t>fragment,theme,null,nullpointerexception,dark-theme,error</t>
+  </si>
+  <si>
+    <t>submission,tolak,dark-theme</t>
+  </si>
+  <si>
+    <t>fragment,orientasi,rotasi,rotate</t>
+  </si>
+  <si>
+    <t>submission,api,recyclerview,fragment,follower,following</t>
+  </si>
+  <si>
+    <t>app-crash,force-close,nullpointerexception</t>
+  </si>
+  <si>
+    <t>terdapat error recyclerview no adapter attached saat menampilkan detail user di fragment follower dan following</t>
+  </si>
+  <si>
+    <t>error recyclerview data tidak tampil di fragment follower dan following</t>
+  </si>
+  <si>
+    <t>recyclerview,no-adapter-attached,fragment,follower,following</t>
+  </si>
+  <si>
+    <t>force close saat kirim data dengan parcelable</t>
+  </si>
+  <si>
+    <t>aplikasi force close saat mengirimkan data ke activity lain dengan parcelable</t>
+  </si>
+  <si>
+    <t>parcelable,activity,force-close</t>
+  </si>
+  <si>
+    <t>error nullpointerexception pada fragment saat ganti jadi dark theme</t>
+  </si>
+  <si>
+    <t>muncul error java lang nullpointerexception pada fragment setelah saya mengganti tema menjadi dark theme</t>
+  </si>
+  <si>
+    <t>dark theme tidak jalan sehingga submission ditolak</t>
+  </si>
+  <si>
+    <t>submission ditolak dengan alasan yang sama yaitu dark theme tidak jalan padahal ketika saya coba dark theme berjalan dengan baik</t>
+  </si>
+  <si>
+    <t>fragment tertutup dan kembali ke fragment awal saat orientasi berubah</t>
+  </si>
+  <si>
+    <t>saya memiliki fragment yang akan memanggil fragment lain namun saat orientasi berubah fragment kedua akan tertutup dan fragment awal akan terpanggil ulang bagaimana cara agar fragment kedua tidak tertutup</t>
+  </si>
+  <si>
+    <t>penggunaan api pada submission</t>
+  </si>
+  <si>
+    <t>apakah api digunakan sebagai data recyclerview atau sebagai data fragment follower following</t>
+  </si>
+  <si>
+    <t>aplikasi force close saat run dengan error androidruntime fatal exception java lang nullpointerexception</t>
+  </si>
+  <si>
+    <t>aplikasi force close saat run nullpointerexception</t>
+  </si>
+  <si>
+    <t>submission ditolak karena implementasi parcelable tidak tepat</t>
+  </si>
+  <si>
+    <t>submission saya ditolak karena pengiriman data antar activity belum memanfaatkan parcelable dengan tepat bagaimana cara mengimplementasikan parcelable dengan tepat</t>
+  </si>
+  <si>
+    <t>parcelable,submission,review,tolak</t>
+  </si>
+  <si>
+    <t>tidak bisa mengirim data ke postman</t>
+  </si>
+  <si>
+    <t>saya coba mengirim data ke api platform postman tapi tidak bisa</t>
+  </si>
+  <si>
+    <t>error,api,postman</t>
+  </si>
+  <si>
+    <t>error recyclerview no adapter saat menggunakan retrofit</t>
+  </si>
+  <si>
+    <t>data dari retrofit muncul di debugger tapi muncul error recyclerview no adapter attached skipping layout sepertinya data dari retrofit tidak masuk ke adapter</t>
+  </si>
+  <si>
+    <t>error,recyclerview,retrofit</t>
+  </si>
+  <si>
+    <t>revisi submission dianggap plagiarisme</t>
+  </si>
+  <si>
+    <t>saya melakukan submission ulang karena terdapat kesalahan di submission sebelumnya namun hasil revisi tersebut ditolak karena plagiarisme saya bahkan membuat project baru untuk mengatasi ini namun selalu ditolak hingga sekarang</t>
+  </si>
+  <si>
+    <t>submission,review,tolak,plagiarisme,plagiarism</t>
+  </si>
+  <si>
+    <t>aplikasi saya force close saat membuka fragment detail berikut errornya java lang illegalargumentexception</t>
+  </si>
+  <si>
+    <t>aplikasi force close ketika membuka detail fragment</t>
+  </si>
+  <si>
+    <t>error,force-close,fragment</t>
+  </si>
+  <si>
+    <t>error saat implementasi room database dengan content provider</t>
+  </si>
+  <si>
+    <t>saya mengalami error saat implementasi room database dengan content provider room database dapat berjalan sebelumnya namun muncul error saat menggunakan content provider</t>
+  </si>
+  <si>
+    <t>error,room,database,content-provider</t>
+  </si>
+  <si>
+    <t>dark theme tidak aktif secara otomatis</t>
+  </si>
+  <si>
+    <t>bagaimana cara agar saat setting set dark theme akan menggunakan dark theme saat membuka aplikasi kembali</t>
+  </si>
+  <si>
+    <t>dark-theme</t>
+  </si>
+  <si>
+    <t>room database error nullpointerexception</t>
+  </si>
+  <si>
+    <t>saya mendapatkan exception ini saat menggunakan room database java lang nullpointerexception attempt to get length of null array</t>
+  </si>
+  <si>
+    <t>error,room,database,null,nullpointerexception</t>
   </si>
 </sst>
 </file>
@@ -84,15 +192,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -100,16 +214,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -118,6 +253,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -392,62 +532,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="32.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="91.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>